<commit_message>
getting repo up to date
</commit_message>
<xml_diff>
--- a/SubRecommender/data/validation_data.xlsx
+++ b/SubRecommender/data/validation_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Competition</t>
   </si>
@@ -94,10 +94,13 @@
     <t>Kaggle Most Popular Improvement</t>
   </si>
   <si>
-    <t>Model Random Improvement</t>
-  </si>
-  <si>
-    <t>Model Most Popular Improvement</t>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Most Popular</t>
+  </si>
+  <si>
+    <t>Our Most Popular Improvement</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -194,6 +197,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -475,183 +487,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J6"/>
+  <dimension ref="B2:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.20703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.26171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.20703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.15625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.3671875" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="49.47265625" customWidth="1"/>
+    <col min="7" max="7" width="8.68359375" customWidth="1"/>
+    <col min="8" max="8" width="25.05078125" customWidth="1"/>
+    <col min="9" max="9" width="29.26171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.15625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="26.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="J2" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>2.2599999999999999E-2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>5.9979999999999999E-2</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.60219</v>
       </c>
-      <c r="G3" s="6">
-        <f>F3/C3</f>
+      <c r="H3" s="6">
+        <f>G3/D3</f>
         <v>26.645575221238939</v>
       </c>
-      <c r="H3" s="6">
-        <f>F3/D3</f>
+      <c r="I3" s="9">
+        <f>G3/E3</f>
         <v>10.039846615538513</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="7" t="s">
+      <c r="J3" s="10">
+        <v>116.44321608040207</v>
+      </c>
+      <c r="K3" s="9">
+        <v>4.8392238809231438</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>4.2110000000000003E-3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>3.1408999999999999E-2</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6">
-        <f>F4/D4</f>
+      <c r="I4" s="9">
+        <f>G4/E4</f>
         <v>7.4587983851816659</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="7" t="s">
+      <c r="J4" s="10">
+        <v>132.28987327609556</v>
+      </c>
+      <c r="K4" s="9">
+        <v>11.871650364524308</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>0.41937999999999998</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>0.49503000000000003</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.73621000000000003</v>
       </c>
-      <c r="G5" s="6">
-        <f>F5/C5</f>
+      <c r="H5" s="6">
+        <f>G5/D5</f>
         <v>1.7554723639658545</v>
       </c>
-      <c r="H5" s="6">
-        <f>F5/D5</f>
+      <c r="I5" s="9">
+        <f>G5/E5</f>
         <v>1.4872027957901541</v>
       </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7" t="s">
+      <c r="J5" s="10">
+        <v>136.84594902322911</v>
+      </c>
+      <c r="K5" s="9">
+        <v>4.6140833454170567</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>2.0000000000000002E-5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>2.0789999999999999E-2</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.17910000000000001</v>
       </c>
-      <c r="G6" s="6">
-        <f>F6/C6</f>
+      <c r="H6" s="6">
+        <f>G6/D6</f>
         <v>8955</v>
       </c>
-      <c r="H6" s="6">
-        <f>F6/D6</f>
+      <c r="I6" s="9">
+        <f>G6/E6</f>
         <v>8.6147186147186154</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="J6" s="10">
+        <v>153.5301045322303</v>
+      </c>
+      <c r="K6" s="9">
+        <v>4.7388376755778587</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" display="https://www.kaggle.com/c/expedia-hotel-recommendations"/>
-    <hyperlink ref="A4" r:id="rId2" display="https://www.kaggle.com/c/santander-product-recommendation"/>
-    <hyperlink ref="A5" r:id="rId3" display="https://www.kaggle.com/c/event-recommendation-engine-challenge"/>
-    <hyperlink ref="A6" r:id="rId4" display="https://www.kaggle.com/c/msdchallenge"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.kaggle.com/c/expedia-hotel-recommendations"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.kaggle.com/c/santander-product-recommendation"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.kaggle.com/c/event-recommendation-engine-challenge"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.kaggle.com/c/msdchallenge"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -663,14 +691,14 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G6" sqref="F2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="10.3125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.47265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.62890625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1015625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.15625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.3671875" bestFit="1" customWidth="1"/>
@@ -681,10 +709,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>21</v>

</xml_diff>